<commit_message>
adição do campo sujeito a ISS, caso exista um item com valor em ISSQN_BLOCO
</commit_message>
<xml_diff>
--- a/output/relatorio_customizado_v3.xlsx
+++ b/output/relatorio_customizado_v3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,10 +536,15 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>Sujeito a ISS?</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>Outros Impostos</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Info Adicionais</t>
         </is>
@@ -651,8 +656,7 @@
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "II_BLOCO": "II"
+      "INFO_ADICIONAL": null
     },
     {
       "NUMERO": "1",
@@ -698,8 +702,7 @@
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "IOF_BLOCO": "IOF"
+      "INFO_ADICIONAL": null
     }
   ],
   "xml_filename": "31230180795727000656550010001320041532351394.xml"
@@ -797,6 +800,11 @@
         </is>
       </c>
       <c r="V2" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||DEVOLUCAO TOTAL REFERENTE NOTA FISCAL Nº 131949 EMITIDA EM 14/01/2023, EM VIRTUDE DE FATURAMENTO INCORRETO . S500 ICMS RETIDO OPER. ANT. P/ REF. BASE DE CALCULO DO ICMS ST R$ 21.592,00 - ICMS ST R$ R$ 3.238,80. GASOLINA COMUM ICMS RETIDO OPER. ANT. P/ REF. BASE DE CALCULO DO ICMS ST R$ 30.117,00 - ICMS ST R$ R$ 5.421,06.||FORMA DE COBRANCA :</t>
         </is>
@@ -908,8 +916,7 @@
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "II_BLOCO": "II"
+      "INFO_ADICIONAL": null
     },
     {
       "NUMERO": "1",
@@ -955,8 +962,7 @@
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "IOF_BLOCO": "IOF"
+      "INFO_ADICIONAL": null
     }
   ],
   "xml_filename": "31230180795727000656550010001320041532351394.xml"
@@ -1050,10 +1056,15 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>IOF</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||DEVOLUCAO TOTAL REFERENTE NOTA FISCAL Nº 131949 EMITIDA EM 14/01/2023, EM VIRTUDE DE FATURAMENTO INCORRETO . S500 ICMS RETIDO OPER. ANT. P/ REF. BASE DE CALCULO DO ICMS ST R$ 21.592,00 - ICMS ST R$ R$ 3.238,80. GASOLINA COMUM ICMS RETIDO OPER. ANT. P/ REF. BASE DE CALCULO DO ICMS ST R$ 30.117,00 - ICMS ST R$ R$ 5.421,06.||FORMA DE COBRANCA :</t>
         </is>
@@ -1144,7 +1155,7 @@
       "ICMS_VICMSST": null,
       "TEM_ICMS": null,
       "TEM_ST": null,
-      "IPI_BLOCO": "teste",
+      "IPI_BLOCO": null,
       "IPI_CST": null,
       "IPI_VBC": null,
       "IPI_PIPI": null,
@@ -1156,17 +1167,16 @@
       "COFINS_PCOFINS": null,
       "COFINS_VCOFINS": null,
       "TEM_COFINS": null,
-      "PIS_BLOCO": "TESTEISSQN",
-      "ISSQN_BLOCO": "TESTEISSQN",
+      "PIS_BLOCO": "PISNT",
+      "ISSQN_BLOCO": null,
       "TEM_ISSQN": null,
-      "OUTRO_IMPOSTO": "IOF",
-      "ICMS_UFDEST_BLOCO": "TESTEISSQN",
+      "OUTRO_IMPOSTO": null,
+      "ICMS_UFDEST_BLOCO": null,
       "ICMS_UFDEST_VBCUFDEST": null,
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "CIDE_BLOCO": "CIDE"
+      "INFO_ADICIONAL": null
     }
   ],
   "xml_filename": "31240180795727000656550010001474151199535000.xml"
@@ -1260,10 +1270,15 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>CIDE, IOF</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS, EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. MOTORISTA REINALDO JOSE CAMPOS JUNIOR, CPF: 12402000643, PLACAS: PEM6F89-PEM6F89-PEM6F89.CONFERI TEOR ALCOOLICO 27%.SAIDA DO PRODUTO ARMAZENADO NA BASE DA FIC DISTRIBUIDORA DE DERIVADOS DE  PETROLEO LTDA. EST. CONTORNO DA PETROBRAS, 1.250 - VILA ESPERANCA - CEP: 32.501-970 - BETIM/MG.AS FISPQ DE TODOS OS PRODUTOS ESTAO DISPONIVEIS NO SITE - WWW.POTENCIAL.NET.BR.GRP. EMBLG. II.RECEBEMOS ENVELOPE DE SEGURANCA PARA AMOSTRA TESTEMUNHA CF RESOLUCAO ANP N.44.NR. ENV. - B1: 6372279 - B2: 6372278 - B3: 6372277 - B4: 6372276||BOLETIM DE CONFORMIDADE No. 11/2024||||||- GASOLINA ICMS MONOF. RET ANT - R$ 12200,00 CONF. CONV. ICMS 15/23 -  -||PROCON BETIM - RUA SAO PEDRO, 42 - CEP 32560-180 - FONE (31) 3531-1188 - FAX (31) 3594-1250 - www.betim.mg.gov.br PROCOM ASSEMBLEIA LEGISLATIVA - RUA CURITIBA, 2002 - BAIRRO LOURDES - BELO HORIZONTE/MG - CEP 30170-122 - FONE (31) 3293-9299 - FAX (31) 3292-7125 - www.almg.gov.br||FORMA DE COBRANCA : BLOQUETO</t>
         </is>
@@ -1375,10 +1390,7 @@
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "II_BLOCO": "II",
-      "IOF_BLOCO": "IOF",
-      "CIDE_BLOCO": "CIDE"
+      "INFO_ADICIONAL": null
     }
   ],
   "xml_filename": "31240180795727000656550010001477411720037863.xml"
@@ -1472,10 +1484,15 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>CIDE, IOF</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||-  - DIESEL ICMS MONOF. RET ANT - R$ 4942,89 CONF. CONV. ICMS 199/22 -||devolução Fic||FORMA DE COBRANCA :</t>
         </is>
@@ -1582,13 +1599,12 @@
       "ISSQN_BLOCO": null,
       "TEM_ISSQN": null,
       "OUTRO_IMPOSTO": null,
-      "ICMS_UFDEST_BLOCO": "ICMSDUFDEST",
+      "ICMS_UFDEST_BLOCO": null,
       "ICMS_UFDEST_VBCUFDEST": null,
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
       "TEM_DIFAL": null,
-      "INFO_ADICIONAL": null,
-      "PMPF_BLOCO": "PMPF"
+      "INFO_ADICIONAL": null
     }
   ],
   "xml_filename": "31240180795727000656550010001481351730889824.xml"
@@ -1682,10 +1698,15 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>PMPF</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||-  -  - B100 ICMS MONOF. RET ANT - R$ 26275,76 CONF. CONV. ICMS 199/22||DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS,EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO.   Placas: BCW8D08 / BBZ0G20 Motorista: MAYK DOUGLAS ARNDT MUNIZ Densidade: 0.879 Temperatura: 30 Densidade corrigida a 20ºc: 879 Temperatura media do(s) compartimento(s): 30 ºC Volume Ambiente: 41.997 Volume Corrigido a 20°c: 41.679 Lacres: 00353019; 00353020; 00353039; 00353040 Nr. Ordem: 0000136442 Nr. Contrato: 0103899000||FORMA DE COBRANCA :</t>
         </is>
@@ -1896,6 +1917,11 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||DEVOLUÇÃO TOTAL REF A NF 500012 EMISSÃO  13/11/2023 ENVITUDE DE PRODUTO ESTÁ FORA DA ESPECIFICAÇÃO||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -2001,7 +2027,7 @@
       "ISSQN_BLOCO": null,
       "TEM_ISSQN": null,
       "OUTRO_IMPOSTO": null,
-      "ICMS_UFDEST_BLOCO": "ICMSDUFDEST",
+      "ICMS_UFDEST_BLOCO": null,
       "ICMS_UFDEST_VBCUFDEST": null,
       "ICMS_UFDEST_PICMSUFDEST": null,
       "ICMS_UFDEST_VICMSUFDEST": null,
@@ -2104,6 +2130,11 @@
         </is>
       </c>
       <c r="V8" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||-  -  - B100 ICMS MONOF. RET ANT - R$ 21271,06 CONF. CONV. ICMS 199/22||ARMAZENAGEM FIC||FORMA DE COBRANCA :</t>
         </is>
@@ -2418,6 +2449,11 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||- GASOLINA ICMS MONOF. RET ANT - R$ 18795,89 CONF. CONV. ICMS 15/23 - DIESEL ICMS MONOF. RET ANT - R$ 116742,78 CONF. CONV. ICMS 199/22 -||armazenagem ale||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -2731,6 +2767,11 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||- GASOLINA ICMS MONOF. RET ANT - R$ 18795,89 CONF. CONV. ICMS 15/23 - DIESEL ICMS MONOF. RET ANT - R$ 116742,78 CONF. CONV. ICMS 199/22 -||armazenagem ale||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -3044,6 +3085,11 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||- GASOLINA ICMS MONOF. RET ANT - R$ 18795,89 CONF. CONV. ICMS 15/23 - DIESEL ICMS MONOF. RET ANT - R$ 116742,78 CONF. CONV. ICMS 199/22 -||armazenagem ale||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -3252,6 +3298,11 @@
         </is>
       </c>
       <c r="V12" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS, EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. MOTORISTA JOSE IZAIAS RODRIGUES DA SILVA, CPF: 31462979653, PLACAS: GWH1263-GWH1263-.CONFERI TEOR ALCOOLICO 27%.GRP. EMBLG. II.RECEBEMOS ENVELOPE DE SEGURANCA PARA AMOSTRA TESTEMUNHA CF RESOLUCAO ANP N.44.NR. ENV. - B4: 6604700||NAF 002076/0001 SMS N PROCESSO 000158/2023 / ATA DE REGISTRO DE PREÇOS Nº 158/2023 - PROCESSO Nº 158/2023 - PREGÃO ELETRÔNICO Nº 043/2023 / BOLETIM DE CONFORMIDADE No. 328/2024||RETENÇÃO DE IRRF DE 0,24% - 4,09 CONFORME DECRETO 066/2023||||- GASOLINA ICMS MONOF. RET ANT - R$ 435,22 CONF. CONV. ICMS 15/23 -  -||PROCON BETIM - RUA SAO PEDRO, 42 - CEP 32560-180 - FONE (31) 3531-1188 - FAX (31) 3594-1250 - www.betim.mg.gov.br PROCOM ASSEMBLEIA LEGISLATIVA - RUA CURITIBA, 2002 - BAIRRO LOURDES - BELO HORIZONTE/MG - CEP 30170-122 - FONE (31) 3293-9299 - FAX (31) 3292-7125 - www.almg.gov.br||FORMA DE COBRANCA : BLOQUETO</t>
         </is>
@@ -3738,6 +3789,11 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -4223,6 +4279,11 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -4708,6 +4769,11 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -5193,6 +5259,11 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -5678,6 +5749,11 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -6163,6 +6239,11 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -6648,6 +6729,11 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||NÃO INCIDÊNCIA DE ICMS CONFORME CAPÍTULO III, ART. 153, XIII, RICMS/2023 DECRETO N 48.589/2023. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 1544 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -6750,7 +6836,7 @@
       "COFINS_VCOFINS": null,
       "TEM_COFINS": null,
       "PIS_BLOCO": "PISNT",
-      "ISSQN_BLOCO": null,
+      "ISSQN_BLOCO": "valeu",
       "TEM_ISSQN": null,
       "OUTRO_IMPOSTO": null,
       "ICMS_UFDEST_BLOCO": null,
@@ -6852,10 +6938,15 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||OPERAÇÃO ISENTA DE ICMS CONFORME ANEXO II, ART. 2, XIII, RICMS/2001 DECRETO N 2.870/2001. RETORNO DE BEM REMETIDO EM COMODATO CONFORME NFE 427 DE 12/12/2023 - ABIX TECNOLOGIA LTDA||FORMA DE COBRANCA :</t>
         </is>
@@ -7066,6 +7157,11 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS, EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. MOTORISTA DANIEL PIRES LOPES, CPF: 06835203692, PLACAS: QXY0J02-QXY0J02-QXY0J05.SAIDA DO PRODUTO ARMAZENADO NA BASE DA FIC DISTRIBUIDORA DE DERIVADOS DE  PETROLEO LTDA. EST. CONTORNO DA PETROBRAS, 1.250 - VILA ESPERANCA - CEP: 32.501-970 - BETIM/MG.AS FISPQ DE TODOS OS PRODUTOS ESTAO DISPONIVEIS NO SITE - WWW.POTENCIAL.NET.BR.GRP. EMBLG. III.RECEBEMOS ENVELOPE DE SEGURANCA PARA AMOSTRA TESTEMUNHA CF RESOLUCAO ANP N.44.NR. ENV. - B2: 6377505||BOLETIM DE CONFORMIDADE No. 431/2024||||||-  - DIESEL ICMS MONOF. RET ANT - R$ 5197,00 CONF. CONV. ICMS 199/22 -||PROCON BETIM - RUA SAO PEDRO, 42 - CEP 32560-180 - FONE (31) 3531-1188 - FAX (31) 3594-1250 - www.betim.mg.gov.br PROCOM ASSEMBLEIA LEGISLATIVA - RUA CURITIBA, 2002 - BAIRRO LOURDES - BELO HORIZONTE/MG - CEP 30170-122 - FONE (31) 3293-9299 - FAX (31) 3292-7125 - www.almg.gov.br||FORMA DE COBRANCA : BLOQUETO</t>
         </is>
       </c>
@@ -7275,6 +7371,11 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS, EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. MOTORISTA SEBASTIAO ABREU FRANCISCO, CPF: 05253382682, PLACAS: RVD3J60-RVD3J60-.DISPENSA DE RECOLHIMENTO ANTECIPADO DO ICMS SOBRE O AEHC - RE/PTA N.16.000178019.89, CONFORME ARTIGO 85, IV, LETRA G DA PARTE GERAL E ARTIGO 46, INCISO I, LETRA B, ITEM 1 E PARAG. 2. INCISO I DO ANEXO XV DO RICMS/2002/MG.SAIDA DO PRODUTO ARMAZENADO NA BASE DA FIC DISTRIBUIDORA DE DERIVADOS DE  PETROLEO LTDA. EST. CONTORNO DA PETROBRAS, 1.250 - VILA ESPERANCA - CEP: 32.501-970 - BETIM/MG.AS FISPQ DE TODOS OS PRODUTOS ESTAO DISPONIVEIS NO SITE - WWW.POTENCIAL.NET.BR.GRP. EMBLG. II.RECEBEMOS ENVELOPE DE SEGURANCA PARA AMOSTRA TESTEMUNHA CF RESOLUCAO ANP N.44.NR. ENV. - B3: 6374595||BOLETIM DE CONFORMIDADE No. 458/2024||||||||PROCON BETIM - RUA SAO PEDRO, 42 - CEP 32560-180 - FONE (31) 3531-1188 - FAX (31) 3594-1250 - www.betim.mg.gov.br PROCOM ASSEMBLEIA LEGISLATIVA - RUA CURITIBA, 2002 - BAIRRO LOURDES - BELO HORIZONTE/MG - CEP 30170-122 - FONE (31) 3293-9299 - FAX (31) 3292-7125 - www.almg.gov.br||FORMA DE COBRANCA : BLOQUETO</t>
         </is>
       </c>
@@ -7483,6 +7584,11 @@
         </is>
       </c>
       <c r="V23" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||ARMAZENAGEM REFERENTE DESC 2505||FORMA DE COBRANCA :</t>
         </is>
@@ -7739,6 +7845,11 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE MATRIZ. MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241. PNEU 275/80/22,5 - LISO FOGO 4956 5150 5198 5199 5481 5484 5485 4332 5333 5334 9033 9034 9035 9036 9037 9038 9040 5641 5841 3620 5051 5008 5009 7377 7406 7407 7410 7417 7421 7422 7637 - PNEU 275/80/22,5 BORRACHUDO FOGO 5155 5157 5161 5164 5166 5492 5493 5326 5327 5328 5329 9053 9054 9055 9045 9046 5090 5091 6579 6587 6588 6589 7433 7435 7685 7687 5758||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -7994,6 +8105,11 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE MATRIZ. MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241. PNEU 275/80/22,5 - LISO FOGO 4956 5150 5198 5199 5481 5484 5485 4332 5333 5334 9033 9034 9035 9036 9037 9038 9040 5641 5841 3620 5051 5008 5009 7377 7406 7407 7410 7417 7421 7422 7637 - PNEU 275/80/22,5 BORRACHUDO FOGO 5155 5157 5161 5164 5166 5492 5493 5326 5327 5328 5329 9053 9054 9055 9045 9046 5090 5091 6579 6587 6588 6589 7433 7435 7685 7687 5758||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -8203,6 +8319,11 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||DEV REF NF 458280 EMISSÃO 20/12/2023 DEVIDO AO ITEM FORA DA ESPECIFICAÇÃO TECNICA||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -8412,6 +8533,11 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||DEVOLUÇÃO TOTAL REF S/NFE 421761-1 DE 29/01/2024 DEVIDO AO MATERIAL INCORRETO||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -8621,6 +8747,11 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS,EMBALADOS, IDENTIFICADOS, E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. MOT CELIO ROBERTO BELARMINO SIQUEIRA CPF 03617311911 - LACRES 6592 6290 6792 5097 6200 6540 5289 6460  - TEMP TQ 20,80 - TEMP OP 26,00 - DEN OP 0,80 - DENS 20 0,8101 - FATOR CONV 0,9989 - LOCAL DE ENTREGA ITAJAI-SC - RDP||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -8830,6 +8961,11 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||VENDA DE SUCATA. DIFERIMENTO DE ICMS CONFORME RICMS/2017, ANEXO VIII, ART.28, I, a), REDUCAO DA CARGA TRIBUTÁRIA EFETIVA DE 19,5% PARA 12%. MERCADORIA TRANSPORTADA POR FERRAGENS COSTA CNPJ 82.010.794/0001-39, MOTORISTA IVONOR JESUS DA COSTA, CPF 530.420.509-04, PLACA MBP0148.||FORMA DE COBRANCA : OUTRAS</t>
         </is>
       </c>
@@ -8932,7 +9068,7 @@
       "COFINS_VCOFINS": null,
       "TEM_COFINS": null,
       "PIS_BLOCO": "PISNT",
-      "ISSQN_BLOCO": null,
+      "ISSQN_BLOCO": "valeu",
       "TEM_ISSQN": null,
       "OUTRO_IMPOSTO": null,
       "ICMS_UFDEST_BLOCO": null,
@@ -9034,10 +9170,15 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||A PEÇA SERÁ ENVIADA VIA MOTO BOY, COLETANDO EM NOSSO FORNECEDOR MASTERTEC E DEIXANDO EM NOSSO FORNECEDOR CAPRIGEM MATRIZ DE CURITIBA.  DEVOLUÇÃO TOTAL REF S/NFE 4375-2 DE 24/04/2024 DEVIDO PEÇA INCORRETA||FORMA DE COBRANCA :</t>
         </is>
@@ -9247,6 +9388,11 @@
         </is>
       </c>
       <c r="V31" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
         <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE AMOSTRA DE UREIA AUTOMOTIVA PARA ANALISE. TRANSPORTE VIA CORREIOS||FORMA DE COBRANCA :</t>
         </is>
@@ -9595,6 +9741,11 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE BETIM. PNEU 275/80/22,5 BORRACHUDO FOGO 10399-10400- 10401-10402- 10403-10404- 10405-10406 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 PNEU 275/80/22,5 LISO FOGO 7374 REFERENTE NFE 785294 MICHELIN DE 30/04/2021 PNEU 275/80/22,5 LISO FOGO 7681-7682 REFERENTE NFE 837918 MICHELIN 15/12/2021 PNEU 275/80/22,5 LISO FOGO 10413-10414-10415-10416-10417-10418- 10419-10420-10421-10422-10423- 10424-10425- 10426-10427-10428-10429-10430-10431-10432 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 - MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241.||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -9942,6 +10093,11 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE BETIM. PNEU 275/80/22,5 BORRACHUDO FOGO 10399-10400- 10401-10402- 10403-10404- 10405-10406 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 PNEU 275/80/22,5 LISO FOGO 7374 REFERENTE NFE 785294 MICHELIN DE 30/04/2021 PNEU 275/80/22,5 LISO FOGO 7681-7682 REFERENTE NFE 837918 MICHELIN 15/12/2021 PNEU 275/80/22,5 LISO FOGO 10413-10414-10415-10416-10417-10418- 10419-10420-10421-10422-10423- 10424-10425- 10426-10427-10428-10429-10430-10431-10432 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 - MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241.||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -10289,6 +10445,11 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE BETIM. PNEU 275/80/22,5 BORRACHUDO FOGO 10399-10400- 10401-10402- 10403-10404- 10405-10406 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 PNEU 275/80/22,5 LISO FOGO 7374 REFERENTE NFE 785294 MICHELIN DE 30/04/2021 PNEU 275/80/22,5 LISO FOGO 7681-7682 REFERENTE NFE 837918 MICHELIN 15/12/2021 PNEU 275/80/22,5 LISO FOGO 10413-10414-10415-10416-10417-10418- 10419-10420-10421-10422-10423- 10424-10425- 10426-10427-10428-10429-10430-10431-10432 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 - MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241.||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -10636,6 +10797,11 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||ENVIO DE PNEUS PARA BASE BETIM. PNEU 275/80/22,5 BORRACHUDO FOGO 10399-10400- 10401-10402- 10403-10404- 10405-10406 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 PNEU 275/80/22,5 LISO FOGO 7374 REFERENTE NFE 785294 MICHELIN DE 30/04/2021 PNEU 275/80/22,5 LISO FOGO 7681-7682 REFERENTE NFE 837918 MICHELIN 15/12/2021 PNEU 275/80/22,5 LISO FOGO 10413-10414-10415-10416-10417-10418- 10419-10420-10421-10422-10423- 10424-10425- 10426-10427-10428-10429-10430-10431-10432 REFERENTE NFE 2518561 BRIDGESTONE 22/02/2024 - MERCADORIA TRANSPORTADA POR POTENCIAL PETROLEO LTDA CNPJ 80.795.727/0001-41 MOTORISTA JEFERSON FERREIRA MARTINS CPF 126.803.756-70 PLACA AZX-5241.||FORMA DE COBRANCA :</t>
         </is>
       </c>
@@ -10845,6 +11011,11 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ||||||||||DEVOLUÇÃO REFERENTE NFE 56996-1 DE 22/12/2023 - MOTIVO DEVIDO O FORMECEDOR ENVIAR O MATERIAL INCORRETO, O QUAL NÃO É MAIS UTILIZADO NA BASE - MERCADORIA SERA TRANSPORTADA PELA TRANSPORTADORA MINUANO LTDA CNPJ: 87.183.570/0022-77-  VALOR TOTAL DO I.P.I. DESTACADO EM NOTA 199,88||FORMA DE COBRANCA :</t>
         </is>
       </c>

</xml_diff>

<commit_message>
adicionando tags IPI e iCMS (+ tabela de-para)
</commit_message>
<xml_diff>
--- a/output/relatorio_customizado_v3.xlsx
+++ b/output/relatorio_customizado_v3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,30 +531,40 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>DESC CST ICMS</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>IPI_CST</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>TIPI</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>CONFINS</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Sujeito a ISS?</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Outros Impostos</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Infos Adicionais</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>DIFAL</t>
         </is>
@@ -755,30 +765,40 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
+          <t>CST 53</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
           <t>ISENTO</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X2" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: DOCUMENTO DE FATURAMENTO 0964553138 SAFRA: 25/26 N DO PEDIDO: POTENCIAL PEDIDO DE COMPRA DO CLIENTE: DCEM20250630130338.4112110 - 000000 PLACA VEICULO: SFC3D69 PR JDG9A12 RS JDG9A14 RS NUMERO DA O.C.:003636/2025 CTRC N . LACRES: 2183396-97-98-99-400-02183101-02-03- TQ06 - CERT ALC 13.2025 - LACRES DE AMOSTRAS 1626069-6070 - AUT 5519969 - AGEND 4664636. AUTORIZACAO CODIF NUM 20250806820801621335 CERTIFICADO DE QUALIDADE N:0000132025 COMERCIALIZACAO DE AEAC ADQUIRIDO DE OUTRO FORNECEDOR INCISO I, ARTIGO 6 DA RESOLUCAO ANP NRO 43/2009 M.ESP= 0,7895 PESOLIQ= 49740.000 SETAVEIC= 63.000,000 FATOR= 0.9984 V.FAT= 62.899 GRAUALC= 99.500 PH= ACIDEZ= 5 CONDUTIV= 20 TEMP.ENS.= 21,5 M.ESP.T.E.= 0.79080 TEMP.VEIC.= 21,5 DIF. VOL.= 0.001- % PRODUTO SERA ENTREGUE, POR NOSSA CONTA E ORDEM, PELA COOPERATIVA PROD DE CANA-DE-ACUCAR , ACUCAR E ALCOOL DO EST S PAULO CNPJ/MF 61149589004176 IE N 480.055.380.111 COM RECOLHIMENTO DIFERIDO CONFORME CONVENIO ICMS 15/2023 ART 419/419B ATO COTEPE 43/2023 PRODUTO NAO TRIBUTADO DE IPI ALIQUOTA 0% - DECRETO N 11.158, DE 2022 | DECLARACAO PARA OS DANFE'S DE EXPEDICAO DE ALCOOL TIPO DOCTO 2: DECLARO QUE OS PRODUTOS PERIGOSOS ESTAO ADEQUADAMENTE CLASSIFICADOS, EMBALADOS, IDENTIFICADOS E ESTIVADOS PARA SUPORTAR OS RISCOS DAS OPERACOES DE TRANSPORTE E QUE ATENDEM AS EXIGENCIAS DA REGULAMENTACAO. N DA ONU:1170 - ETANOL ALCOOL ETILICO CLASSE 3 - GRUPO EMBALAGEM. II - ALCOOL CORRIGIDO A 20 C. ORIGEM DA MATERIA PRIMA: CANA DE ACUCAR | ESCRITORIO CENTRAL SP: AV. DAS NACOES UNIDAS,14261 ALA A1 12 13 SAO PAULO - SP - CEP: 04794-000 - TEL: 0112618-8166 | [ITEM 1]: M.Esp= 0,7895 PesoLiq= 49740.000 SetaVeic= 63.000,000 Fator= 0.9984 V.Fat= 62.899 GrauAlc= 99.500 PH= Acidez= 5 Condutiv= 20 Temp.Ens.= 21,5 M.Esp.T.E.= 0.79080 Temp.Veic.= 21,5 Dif. Vol.= 0.001- % Produto será entregue, por nossa conta e ordem, pela Cooperativa Prod de Cana-de-Açúcar , Açúcar e Álcool do Est S Paulo CNPJ/MF 61149589004176 IE Nº 480.055.380.111 com recolhimento diferido conforme convênio ICMS 15/2023 Art 419/419B Ato Cotepe 43/2023</t>
         </is>
       </c>
-      <c r="Y2" t="b">
+      <c r="AA2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -977,30 +997,40 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
+          <t>CST 53</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
           <t>ISENTO</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X3" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: Placas: SED7D22 / RYF3A40 / RYF3A50 Motorista: CLEBERSON VAZ DE CARVALHAES Densidade: 0.8789 Temperatura: 24.0 Densidade corrigida a 20(o)c: 878.9 Temperatura media do(s) compartimento(s): 23.7 (o)C Volume Ambiente: 60.012 Volume Corrigido a 20oc: 59.845 Lacres: 0517609; 0517610; 0517611; 0517612; 0517613; 0517614; 0517615; 0517616 Numero do certificado: 0114 / 2025 Numero do tanque: 1409 Lacres da amostra testemunho: 0109379-0109380 ICMS monofasico sobre combustiveis dif conf Conv ICMS 199/2022 IPI nao tributado conforme capitulo 38 da tabela TIPI</t>
         </is>
       </c>
-      <c r="Y3" t="b">
+      <c r="AA3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1199,30 +1229,40 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
+          <t>Com redução da base de cálculo</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
           <t>ISENTO</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X4" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: BC REDUZIDA EM 38% CFE. ART. 4 -D na Resolucao do CONDEPRODEMAT n 040/2019 C.C ART. 14 DA LC 798/2024. NOS TERMOS DO 1 DO ARTIGO 35 DA LC N 631/2019 A FRUICAO DO BENEFICIO FISCAL PREVISTO NESTE ARTIGO ENCERRA A CADEIA TRIBUTARIA RELATIVA AO PRODUTO ACIDEZ TOTAL 9,69 CONDUTIVIDADE 105,00 PH 6,40 HORA ANAlISE 15:00 N CERTIFICADO 163 DT ANALISE 05/02/2025 MASSA ESPECIFICA 20 809,80 Temp. veiculo: 20,00 Cap. Seta: 76.236 Vol. Faturado: 76.236,000 Grau INPM: 93,00 Massa Especifica a 20 : 809,80 Massa Especifica: 0,8054 Fator de reducao: 1,0000 CHAMADO: 369941 LACRE(S): 1 Placa POT0808 PEDIDO INTERNO: 125052 | [ITEM 1]: FINS CARBURANTE</t>
         </is>
       </c>
-      <c r="Y4" t="b">
+      <c r="AA4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1421,30 +1461,40 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
+          <t>Tributada integralmente</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
           <t>ISENTO</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X5" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: ICMS tributado conforme previsao do art. 41, I do RICMS/MS. SAIDA NAO TRIBUTADA IPI NOS TERMOS DO DEC. 8.950/16** **ICMS TRIBUTADO CONFORME PREVISAO DO ART. 41, I DO RICMS/MS.**SAIDA NAO TRIBUTADA IPI NOS TERMOS DO DEC. 8. 950/16**HIDRATADO: LACRE AMOSTRA TESTEMUNHA CARRETA: 2932999 LACRE ANP 2932433/2932434 CERTIFICADO ANP 202522..N  CERTIFICADO LAUDO:201621592 PAMCARY 24 HORAS ACIDENTE E ROUBO 0800-7404-000 (11) 3889- 1000..**DESCRICAO LONGA DO PRODUTO: 200870 - COMBUSTIVEL LIQUIDO..TIPO COMBUSTIVEL: ETANOL.CARACTERISTICAS ADICIONAIS: CLASSE OU SUBCLASSE RISCO 3 - GRUPO EMBALAGEM II, DESCRICAO CLASSE OU SUBCLASSE RISCO - LIQUIDOINFLAMAVEL, NUMERO ONU 1170, NUMERO RISCO 33,.DECLARO QUE O PRODUTO ESTA ADEQUADAMENTE CLASSIFICADO, EMBALADO, IDENTIFICADO E ESTIVADO PARA SUPORTAR OS RISCOS DAS OPERACOESTRANSPORTE E QUE ATENDE AS EXIGENCIAS DA REGULAMENTACAO - RESOLUCAO ANTT 5998/2022.COMPLEMENTO: HIDRATADO**N  DA ORDEM DE COMPRA: 1 S AGOSTO 25**LOCAL DE ENTREGA: SADIPE SERV AUX DE DISTRIB DE PE TROLEO - CNPJ/CPF: 00711620000139 - ENDERECO: RUA DOUTOR ELI VOLPATO , N.O: 948 - BAIRRO: CHAPADA - CIDADE: ARAUCARIA - CEP: PR 4101804 - UF: PR**PEDIDO DE VENDA: 0000186432**N  CONTRATO: 0000000451**COD. ANP: 810101001**LACRES: 2947636 2947635 2947634 2947633 2947640 2947639 2947638 2947637**MOTORISTA: JOSE CARLOS PASSIANOTO BATISTA CPF DO MOTORISTA: 97914509191**PLACA DO VEICULO: SMF9J73 UF: MS**PLACA REBOQUE : OOM5E83 UF: MS ** PLACA REBOQUE : OOM5F62 UF: MS COD. ANP: 810101001</t>
         </is>
       </c>
-      <c r="Y5" t="b">
+      <c r="AA5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1643,30 +1693,40 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
+          <t>CST 15</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
           <t>SEM_IPI</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X6" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: TRIBUTACAO MONOFASICA PROPRIA E COM RESPONSABILIDADE PELA *RETENCAO SOBRE COMBUSTIVEIS. *IMUNIDADE DO IPI - CONF.ART.155, p 3o., DA CONST. FED. DE 88, *E CONF. INCISO IV, ARTIGO 18 DO DECRETO No 7.212/2010. * I.B.:L295202505715. Cert.Ensaio:1602/2025/295. * 1400 *Modalidade de venda:EXA *Tipo de contrato:N4 *Ordem:0224293438 *Quantidade referente a 20o C e densidade 0.7295 RH2 *Volume referido a temperatura ambiente:399734litros *Valor unitario referente a volume contratual: R5.183400/Litro. * Local de Entrega: SADIPE-SERVICOS AUXILIARES R DOUTOR ELI VOLPATO S/N CHAPADA ARAUCARIA PR CEP.: 83707-746 Inscricao Estadual 9032100101 CNPJ 00711620000139 | [ITEM 1]: ONU 1203, COMBUSTIVEL PARA MOTORES, Classe 3, GE II *ICMS monofasico proprio: BC: 398.215,0000 Litro Aliquota: R 1,4700 ICMS Mono: R 585.376,05 ICMS monofasico sujeito a retencao: BC: 170.663,5714 Litro Aliquota: R 1,4700 ICMS Mono: R 250.875,45</t>
         </is>
       </c>
-      <c r="Y6" t="b">
+      <c r="AA6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1865,30 +1925,40 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
+          <t>CST 15</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
           <t>SEM_IPI</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>NAO</t>
-        </is>
-      </c>
       <c r="X7" t="inlineStr">
         <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>NAO</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
           <t>[CONTRIBUINTE]: TRIBUTACAO MONOFASICA PROPRIA E COM RESPONSABILIDADE PELA *RETENCAO SOBRE COMBUSTIVEIS. *IMUNIDADE DO IPI - CONF.ART.155, p 3o., DA CONST. FED. DE 88, *E CONF. INCISO IV, ARTIGO 18 DO DECRETO No 7.212/2010. * I.B.:L295202505682. Cert.Ensaio:1585/2025/295. * 1400 *Modalidade de venda:EXA *Tipo de contrato:N4 *Ordem:0224289242 *Quantidade referente a 20o C e densidade 0.8438 RH2 *Volume referido a temperatura ambiente:734095litros *Valor unitario referente a volume contratual: R4.681400/Litro. * Local de Entrega: SADIPE-SERVICOS AUXILIARES R DOUTOR ELI VOLPATO S/N CHAPADA ARAUCARIA PR CEP.: 83707-746 Inscricao Estadual 9032100101 CNPJ 00711620000139 | [ITEM 1]: ONU 1202, OLEO DIESEL, Classe 3 , GE III *ICMS monofasico proprio: BC: 732.627,0000 Litro Aliquota: R 1,1200 ICMS Mono: R 820.542,24 ICMS monofasico sujeito a retencao: BC: 129.287,1176 Litro Aliquota: R 1,1200 ICMS Mono: R 48.262,36</t>
         </is>
       </c>
-      <c r="Y7" t="b">
+      <c r="AA7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>